<commit_message>
Added capability to put multiple emails
Added capability to put multiple emails separated by comma
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -11,24 +11,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+  <si>
+    <t>User ID</t>
   </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>2021-02-22</t>
+    <t>Phone Number(s)</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Department Name</t>
+  </si>
+  <si>
+    <t>Shah Hossain</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Husna Zaman Al Hadi</t>
+  </si>
+  <si>
+    <t>Md. Azaj Ikbal</t>
   </si>
   <si>
     <t>M Nahid Al Fuad</t>
@@ -37,13 +46,115 @@
     <t>Support</t>
   </si>
   <si>
-    <t>15:08:29</t>
+    <t>Musfeq Noor Afsar</t>
+  </si>
+  <si>
+    <t>Saif Chowdhury</t>
+  </si>
+  <si>
+    <t>Sudip Majumder</t>
+  </si>
+  <si>
+    <t>Md. Firoz Hossain Khan</t>
+  </si>
+  <si>
+    <t>Nafisa Binte Amin</t>
+  </si>
+  <si>
+    <t>Accounts_&amp;_Admin</t>
+  </si>
+  <si>
+    <t>Tareq Naushad</t>
+  </si>
+  <si>
+    <t>CTO</t>
+  </si>
+  <si>
+    <t>Anika Nawar Wahid</t>
+  </si>
+  <si>
+    <t>US_Back_Office</t>
+  </si>
+  <si>
+    <t>Md Mozammel Hossain</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Md. Razib Hasan</t>
+  </si>
+  <si>
+    <t>Saikat</t>
+  </si>
+  <si>
+    <t>App_Development</t>
   </si>
   <si>
     <t>Sayed</t>
   </si>
   <si>
-    <t>15:03:32</t>
+    <t>Jamshed</t>
+  </si>
+  <si>
+    <t>System_Admin</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Marketing_</t>
+  </si>
+  <si>
+    <t>Farhan</t>
+  </si>
+  <si>
+    <t>Ihtesham</t>
+  </si>
+  <si>
+    <t>Mashrur</t>
+  </si>
+  <si>
+    <t>Maahdi M</t>
+  </si>
+  <si>
+    <t>HR_&amp;_Admin</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Md.Hosen</t>
+  </si>
+  <si>
+    <t>Nusrath</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>Rotna</t>
+  </si>
+  <si>
+    <t>Rizvi</t>
+  </si>
+  <si>
+    <t>01734189710</t>
+  </si>
+  <si>
+    <t>r17v1.hasan@gmail.com</t>
+  </si>
+  <si>
+    <t>Md. Kamruzzaman</t>
+  </si>
+  <si>
+    <t>M. Sakib Hussain</t>
+  </si>
+  <si>
+    <t>8888</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -430,7 +541,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E32"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="25" style="1" customWidth="1"/>
@@ -454,38 +565,395 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>33</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>34</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>1002</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>1004</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>5001</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>5003</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>8888</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>9999</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>